<commit_message>
feat: Adecuacion Historial Academico
</commit_message>
<xml_diff>
--- a/web/resources/uploads/historial_academico.xlsx
+++ b/web/resources/uploads/historial_academico.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t xml:space="preserve">Código de registro:</t>
   </si>
@@ -68,43 +68,22 @@
     <t xml:space="preserve">&lt;&lt;CONCLUSION&gt;&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">MENCIÓN:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;&lt;MENCION&gt;&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">NIVEL DE FORMACIÓN:</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;&lt;NIVEL_ACADEMICO&gt;&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">REGIMEN:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;&lt;REGIMEN&gt;&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">N°</t>
   </si>
   <si>
-    <t xml:space="preserve">LIBRO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FOLIO</t>
-  </si>
-  <si>
     <t xml:space="preserve">GESTIÓN ACADÉMICA</t>
   </si>
   <si>
-    <t xml:space="preserve"> SEMESTRE/ AÑO</t>
-  </si>
-  <si>
     <t xml:space="preserve">CÓDIGO</t>
   </si>
   <si>
-    <t xml:space="preserve">ASIGNATURA</t>
+    <t xml:space="preserve">MODULO</t>
   </si>
   <si>
     <t xml:space="preserve">PRE REQUISITO</t>
@@ -119,22 +98,13 @@
     <t xml:space="preserve">OBSERVACIONES</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;&lt;LIBRO&gt;&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;&lt;FOLIO&gt;&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;&lt;GA&gt;&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;&lt;NIVEL&gt;&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;&lt;CODIGO&gt;&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;&lt;MATERIA&gt;&gt;</t>
+    <t xml:space="preserve">&lt;&lt;MODULO&gt;&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;&lt;COD_PRE&gt;&gt;</t>
@@ -143,19 +113,10 @@
     <t xml:space="preserve">&lt;&lt;CONDICION&gt;&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Lugar y fecha:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;&lt;LUGAR_FECHA&gt;&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;&lt;RM_1&gt;&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;&lt;RM_2&gt;&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;&lt;RM_3&gt;&gt;</t>
+    <t xml:space="preserve">Fecha:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;FECHA&gt;&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Firma de autoridad académica</t>
@@ -170,7 +131,7 @@
     <t xml:space="preserve">Carga Horaria</t>
   </si>
   <si>
-    <t xml:space="preserve">61 a 100</t>
+    <t xml:space="preserve">80 a 100</t>
   </si>
   <si>
     <t xml:space="preserve">APROBADO</t>
@@ -182,7 +143,7 @@
     <t xml:space="preserve">&lt;&lt;MA_MC&gt;&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">0 a 60</t>
+    <t xml:space="preserve">0 a 80</t>
   </si>
   <si>
     <t xml:space="preserve">REPROBADO</t>
@@ -361,7 +322,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -458,10 +419,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -474,8 +431,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -762,35 +719,34 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:N31"/>
+  <dimension ref="A2:N26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55859375" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="48.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="6.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="3.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="13.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="48.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="6.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="3.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="1" width="10.16"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="4" t="n">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="4" t="n">
         <v>-1</v>
       </c>
     </row>
@@ -806,9 +762,6 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6"/>
@@ -820,47 +773,38 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8" t="s">
+      <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="9"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11" t="n">
+      <c r="B7" s="11" t="n">
         <v>-2</v>
       </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12" t="s">
+      <c r="F7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="13" t="s">
+      <c r="G7" s="6"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="13" t="s">
         <v>6</v>
       </c>
     </row>
@@ -868,21 +812,18 @@
       <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="14" t="s">
+      <c r="B8" s="14" t="s">
         <v>8</v>
       </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="15" t="s">
+      <c r="F8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="16"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="13" t="s">
+      <c r="G8" s="16"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="13" t="s">
         <v>10</v>
       </c>
     </row>
@@ -890,370 +831,257 @@
       <c r="A9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11" t="s">
+      <c r="B9" s="11" t="s">
         <v>12</v>
       </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="15" t="s">
+      <c r="F9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="16"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="13" t="s">
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11" t="s">
+      <c r="B10" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="s">
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" s="21" customFormat="true" ht="10.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="14" t="s">
+      <c r="B11" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="6"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="s">
+      <c r="C11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="14" t="s">
+      <c r="D11" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-    </row>
-    <row r="13" s="21" customFormat="true" ht="10.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18" t="s">
+      <c r="E11" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="F11" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="G11" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="H11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="I11" s="18"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="18"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="C13" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="D13" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="E13" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I13" s="20" t="s">
+      <c r="F13" s="22" t="n">
+        <v>-50</v>
+      </c>
+      <c r="G13" s="22" t="n">
+        <v>-51</v>
+      </c>
+      <c r="H13" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="I13" s="22"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="18" t="s">
+      <c r="B15" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="L13" s="18"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="22" t="n">
-        <v>-3</v>
-      </c>
-      <c r="B15" s="22" t="s">
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="24"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="24"/>
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="D20" s="29"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="B22" s="30"/>
+      <c r="C22" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="D22" s="31"/>
+      <c r="E22" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="33" t="n">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="B23" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="I15" s="22" t="n">
-        <v>-50</v>
-      </c>
-      <c r="J15" s="22" t="n">
-        <v>-51</v>
-      </c>
-      <c r="K15" s="22" t="s">
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="L15" s="22"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="24"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="25"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="27" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="E17" s="1" t="s">
+      <c r="B24" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="25"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E18" s="24"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="25"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="28" t="s">
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="24"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="28" t="s">
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="22" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="34" t="n">
+        <v>80</v>
+      </c>
+      <c r="B25" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="24"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="28" t="s">
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="22"/>
+    </row>
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="28"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="24"/>
-    </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="29"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="34" t="n">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="35"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="35"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="22" t="n">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="35" t="n">
-        <v>61</v>
-      </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="35"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="33"/>
-      <c r="L30" s="22"/>
-    </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="29"/>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="36"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="36"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="D12:H12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="E27:G30"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="H29:K30"/>
-    <mergeCell ref="L29:L30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E31:G31"/>
+  <mergeCells count="24">
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D25"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="E23:H23"/>
+    <mergeCell ref="E24:H25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="C26:D26"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1276,7 +1104,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55859375" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>